<commit_message>
已修改        Documentation~/Sample.xlsx 已修改        Editor/ExcelHelper.cs 已修改        Editor/LanguagePacker.cs 已修改        Runtime/LocalizationManager.cs
</commit_message>
<xml_diff>
--- a/Documentation~/Sample.xlsx
+++ b/Documentation~/Sample.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4FE836-8E62-41D1-B4C1-C74EC8E6E80B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37315D1A-5DA0-430E-A4FD-B0DE57621263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>GameName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -287,6 +287,63 @@
   </si>
   <si>
     <t>「{GameName}」&lt;color=orange&gt;を使う前に充電&lt;/color&gt;しておいてください。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dialog0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TextName 如果是“^”则表示沿用前一行 TextName 的前缀并自动递增后缀的编号，这就是自动编号功能。这要求一系列自动编号的第一个必须明确指定前缀和初始后缀编号。使用这个功能的好处是，在对行进行插入、删除或者调整顺序时不必手动修改 TextName 来保证编号连续，程序也可以通过循环遍历的方式来访问这些行。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这是一系列自动编号的第一个。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If the TextName is "^", it means that it inherits the prefix of the previous line TextName and automatically increments the number of the suffix. This is the automatic numbering function. This requires that the first of a series of automatic numbering must explicitly specify the prefix and initial suffix number. The advantage of using this function is that you don't have to manually modify the TextName when inserting, deleting, or adjusting the order to ensure that the numbers are continuous. The program can also access these rows through a loop.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This is the first in a series of automatic numbering.</t>
+  </si>
+  <si>
+    <t>The final TextName of this line will be "Dialog1".</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The final TextName of this line will be "Dialog2".</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TextNameが「^」の場合、前の行のTextNameのプレフィックスを継承し、サフィックスの番号を自動的にインクリメントすることを意味します。これは自動番号付け機能です。 これには、一連の自動番号付けの最初で、プレフィックスと初期サフィックス番号を明示的に指定する必要があります。 この関数を使用する利点は、番号が連続するように順序を挿入、削除、または調整するときにTextNameを手動で変更する必要がないことです。また、プログラムはループを介してこれらの行にアクセスできます。</t>
+  </si>
+  <si>
+    <t>これは一連の自動番号付けの最初のものです。</t>
+  </si>
+  <si>
+    <t>这一行的实际 TextName 会是“Dialog1”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这一行的实际 TextName 会是“Dialog2”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>この行の最後のTextNameは「Dialog1」になります。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>この行の最後のTextNameは「Dialog2」になります。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This is the first in a series of automatic numbering.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -738,18 +795,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B31" sqref="B31"/>
+      <selection pane="topRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="67.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="56.625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55.875" style="4" customWidth="1"/>
     <col min="4" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
@@ -933,6 +990,47 @@
       </c>
       <c r="C25" s="4" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="B27" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -944,11 +1042,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8AE7C58-882C-4B75-B7CB-D99F613C0896}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D25" sqref="D25"/>
+      <selection pane="topRight" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1150,6 +1248,47 @@
         <v>45</v>
       </c>
     </row>
+    <row r="27" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>